<commit_message>
Ajout du nom de projet
</commit_message>
<xml_diff>
--- a/Timesheet-Groupe_8.xlsx
+++ b/Timesheet-Groupe_8.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="973" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Groupe" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,34 +28,42 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Groupe!$B$1:$W$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Groupe!$B$1:$W$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">Groupe!$B$1:$W$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">Groupe!$B$1:$W$27</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="Z_DEF7657E_CF5E_43E5_870D_F4B63193E461_.wvu.Cols" vbProcedure="false">'Etudiant 1'!$A:$A</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'Etudiant 1'!$B$1:$T$23</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0" vbProcedure="false">'Etudiant 1'!$B$1:$T$23</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Etudiant 1'!$B$1:$T$23</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="Z_DEF7657E_CF5E_43E5_870D_F4B63193E461_.wvu.Cols" vbProcedure="false">'Etudiant 2'!$A:$A</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">'Etudiant 2'!$B$1:$T$23</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0" vbProcedure="false">'Etudiant 2'!$B$1:$T$23</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Etudiant 2'!$B$1:$T$23</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="Z_DEF7657E_CF5E_43E5_870D_F4B63193E461_.wvu.Cols" vbProcedure="false">'Etudiant 3'!$A:$A</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'Etudiant 3'!$B$1:$T$23</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0" vbProcedure="false">'Etudiant 3'!$B$1:$T$23</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Etudiant 3'!$B$1:$T$23</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="Z_DEF7657E_CF5E_43E5_870D_F4B63193E461_.wvu.Cols" vbProcedure="false">'Etudiant 4'!$A:$A</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area" vbProcedure="false">'Etudiant 4'!$B$1:$T$23</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0" vbProcedure="false">'Etudiant 4'!$B$1:$T$23</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Etudiant 4'!$B$1:$T$23</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="Z_DEF7657E_CF5E_43E5_870D_F4B63193E461_.wvu.Cols" vbProcedure="false">'Etudiant 5'!$A:$A</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm.Print_Area" vbProcedure="false">'Etudiant 5'!$B$1:$T$23</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm.Print_Area_0" vbProcedure="false">'Etudiant 5'!$B$1:$T$23</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Etudiant 5'!$B$1:$T$23</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="Z_DEF7657E_CF5E_43E5_870D_F4B63193E461_.wvu.Cols" vbProcedure="false">'Etudiant 6'!$A:$A</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'Etudiant 6'!$B$1:$T$23</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area_0" vbProcedure="false">'Etudiant 6'!$B$1:$T$23</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Etudiant 6'!$B$1:$T$23</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="Z_DEF7657E_CF5E_43E5_870D_F4B63193E461_.wvu.Cols" vbProcedure="false">'Etudiant 7'!$A:$A</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area" vbProcedure="false">'Etudiant 7'!$B$1:$T$23</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0" vbProcedure="false">'Etudiant 7'!$B$1:$T$23</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Etudiant 7'!$B$1:$T$23</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="38">
   <si>
     <t>Date</t>
   </si>
@@ -63,16 +71,16 @@
     <t>Prévision (charge/semaine)</t>
   </si>
   <si>
-    <t>Restitution </t>
+    <t>Restitution</t>
   </si>
   <si>
-    <t>Etudes </t>
+    <t>Etudes</t>
   </si>
   <si>
-    <t>Réalisation </t>
+    <t>Réalisation</t>
   </si>
   <si>
-    <t>Validation </t>
+    <t>Validation</t>
   </si>
   <si>
     <t>Suivi</t>
@@ -96,7 +104,7 @@
     <t>Maquette</t>
   </si>
   <si>
-    <t>Déploiement </t>
+    <t>Déploiement</t>
   </si>
   <si>
     <t>Etudes des besoins</t>
@@ -108,7 +116,7 @@
     <t>Choix critères qualité</t>
   </si>
   <si>
-    <t>Conception / Modélisation </t>
+    <t>Conception / Modélisation</t>
   </si>
   <si>
     <t>Définition des plans de tests</t>
@@ -129,7 +137,7 @@
     <t>Documentation utilisateur</t>
   </si>
   <si>
-    <t>Tests unitaires </t>
+    <t>Tests unitaires</t>
   </si>
   <si>
     <t>Tests fonctionnels</t>
@@ -145,6 +153,9 @@
   </si>
   <si>
     <t>Nom du produit :</t>
+  </si>
+  <si>
+    <t>ProjetFramboise</t>
   </si>
   <si>
     <t>Nom :</t>
@@ -1334,19 +1345,19 @@
   <dimension ref="A1:W27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="AB35" activeCellId="0" sqref="AB35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.4251012145749"/>
-    <col collapsed="false" hidden="false" max="20" min="4" style="0" width="6.57085020242915"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="10.5748987854251"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="14.7125506072875"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="31"/>
-    <col collapsed="false" hidden="false" max="1025" min="24" style="0" width="10.5748987854251"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.8520408163265"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.4234693877551"/>
+    <col collapsed="false" hidden="false" max="20" min="4" style="0" width="6.57142857142857"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="10.5765306122449"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="14.7142857142857"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="31.0051020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="24" style="0" width="10.5765306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1569,7 +1580,7 @@
       </c>
       <c r="W4" s="29"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="21" t="n">
         <f aca="false">A4+7</f>
         <v>42261</v>
@@ -3253,7 +3264,9 @@
       <c r="B27" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="49"/>
+      <c r="C27" s="49" t="s">
+        <v>30</v>
+      </c>
       <c r="D27" s="49"/>
       <c r="E27" s="49"/>
       <c r="F27" s="49"/>
@@ -3561,9 +3574,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="19" min="3" style="0" width="6.57085020242915"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="10.5748987854251"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.8520408163265"/>
+    <col collapsed="false" hidden="false" max="19" min="3" style="0" width="6.57142857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="10.5765306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4294,10 +4307,10 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="48" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C23" s="49" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D23" s="49"/>
       <c r="E23" s="49"/>
@@ -4352,9 +4365,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="19" min="3" style="0" width="6.57085020242915"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="10.5748987854251"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.8520408163265"/>
+    <col collapsed="false" hidden="false" max="19" min="3" style="0" width="6.57142857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="10.5765306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5085,10 +5098,10 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="48" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C23" s="49" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D23" s="49"/>
       <c r="E23" s="49"/>
@@ -5143,9 +5156,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="19" min="3" style="0" width="6.57085020242915"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="10.5748987854251"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.8520408163265"/>
+    <col collapsed="false" hidden="false" max="19" min="3" style="0" width="6.57142857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="10.5765306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5876,10 +5889,10 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="48" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C23" s="49" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D23" s="49"/>
       <c r="E23" s="49"/>
@@ -5934,9 +5947,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="19" min="3" style="0" width="6.57085020242915"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="10.5748987854251"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.8520408163265"/>
+    <col collapsed="false" hidden="false" max="19" min="3" style="0" width="6.57142857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="10.5765306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6667,10 +6680,10 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="48" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C23" s="49" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D23" s="49"/>
       <c r="E23" s="49"/>
@@ -6725,9 +6738,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="19" min="3" style="0" width="6.57085020242915"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="10.5748987854251"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.8520408163265"/>
+    <col collapsed="false" hidden="false" max="19" min="3" style="0" width="6.57142857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="10.5765306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7458,10 +7471,10 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="48" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C23" s="49" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D23" s="49"/>
       <c r="E23" s="49"/>
@@ -7516,9 +7529,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="19" min="3" style="0" width="6.57085020242915"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="10.5748987854251"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.8520408163265"/>
+    <col collapsed="false" hidden="false" max="19" min="3" style="0" width="6.57142857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="10.5765306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8249,10 +8262,10 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="48" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C23" s="49" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D23" s="49"/>
       <c r="E23" s="49"/>
@@ -8307,9 +8320,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="19" min="3" style="0" width="6.57085020242915"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="10.5748987854251"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.8520408163265"/>
+    <col collapsed="false" hidden="false" max="19" min="3" style="0" width="6.57142857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="10.5765306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9038,7 +9051,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="48" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C23" s="49"/>
       <c r="D23" s="49"/>

</xml_diff>